<commit_message>
updates on data validation and scripts examination
</commit_message>
<xml_diff>
--- a/geocoding/affiliate_network_list_20250401.xlsx
+++ b/geocoding/affiliate_network_list_20250401.xlsx
@@ -30,7 +30,7 @@
     <sheet name="Genomics of the Brazilian Biodiversity (GBB)" sheetId="21" state="visible" r:id="rId21"/>
     <sheet name="Dresden HQ Genomes Project" sheetId="22" state="visible" r:id="rId22"/>
     <sheet name="EBP-Norway" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet name="Cetacean Genomes Project" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="Cetaceans Genomes Project" sheetId="24" state="visible" r:id="rId24"/>
     <sheet name="Darwin Tree of Life (DTOL)" sheetId="25" state="visible" r:id="rId25"/>
     <sheet name="1,000 Bat Genomes (Bat1K)" sheetId="26" state="visible" r:id="rId26"/>
     <sheet name="An Atlas of Eukaryotic Marine Genomes (ATLASea)" sheetId="27" state="visible" r:id="rId27"/>
@@ -3879,7 +3879,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Cetacean Genomes Project (CGP)</t>
+          <t>Cetaceans Genomes Project (CGP)</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -3912,7 +3912,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Cetacean Genomes Project (CGP)</t>
+          <t>Cetaceans Genomes Project (CGP)</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -3945,7 +3945,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Cetacean Genomes Project (CGP)</t>
+          <t>Cetaceans Genomes Project (CGP)</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -3978,7 +3978,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Cetacean Genomes Project (CGP)</t>
+          <t>Cetaceans Genomes Project (CGP)</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -4011,7 +4011,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Cetacean Genomes Project (CGP)</t>
+          <t>Cetaceans Genomes Project (CGP)</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -4044,7 +4044,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Cetacean Genomes Project (CGP)</t>
+          <t>Cetaceans Genomes Project (CGP)</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -4077,7 +4077,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Cetacean Genomes Project (CGP)</t>
+          <t>Cetaceans Genomes Project (CGP)</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -8478,11 +8478,15 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Calle 72 #12 - 65 Piso 7, Chapinero, Bogotá, Cundinamarca, Colombia</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
+          <t>Calle 72 - 65 Piso 7, Chapinero, Bogotá, Cundinamarca, Colombia</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>4.6535353</v>
+      </c>
+      <c r="G3" t="n">
+        <v>-74.05484229999999</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">

</xml_diff>